<commit_message>
included supplemental material file
</commit_message>
<xml_diff>
--- a/docs/manifest.xlsx
+++ b/docs/manifest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhavesh\Documents\SODA Manifest Files\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhavesh\Documents\GitHub\GI-review-dataset\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B339785-3ADB-40B2-8F69-118136AF13E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5418D0-8401-43AE-B9E9-713374B42B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2925" yWindow="1605" windowWidth="23760" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>filename</t>
   </si>
@@ -43,10 +43,22 @@
     <t>2021-09-08T12:28:05,916491-07:00</t>
   </si>
   <si>
+    <t>.xlsx</t>
+  </si>
+  <si>
+    <t>supplemental.pdf</t>
+  </si>
+  <si>
+    <t>2021-09-07T12:04:41,040177-07:00</t>
+  </si>
+  <si>
+    <t>Contains supplementary paragraphs and  tables referred in our paper</t>
+  </si>
+  <si>
+    <t>.pdf</t>
+  </si>
+  <si>
     <t>Multiple information was extracted from the reviewed studies to conduct our analysis, including title, publication year, species for the source of the tissue, test protocol, model category, etc. All results from the review have been stored this spreadsheet. It also includes a glossary of the technical terms used to characterize and classify the different studies in the review.</t>
-  </si>
-  <si>
-    <t>.xlsx</t>
   </si>
 </sst>
 </file>
@@ -410,15 +422,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -446,10 +460,24 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>